<commit_message>
scale to state of the art
</commit_message>
<xml_diff>
--- a/docs/planning.xlsx
+++ b/docs/planning.xlsx
@@ -1189,26 +1189,26 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="4" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1835,7 +1835,7 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp2.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Spin" dx="16" fmlaLink="período_selecionado" max="60" min="1" page="10" val="51"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Spin" dx="16" fmlaLink="período_selecionado" max="60" min="1" page="10" val="55"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3053,7 +3053,7 @@
       <pane xSplit="8" ySplit="5" topLeftCell="I6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="I1" sqref="I1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
-      <selection pane="bottomRight" activeCell="BD38" sqref="BD38"/>
+      <selection pane="bottomRight" activeCell="AH39" sqref="AH39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.75" defaultRowHeight="17.25" x14ac:dyDescent="0.3"/>
@@ -3100,7 +3100,7 @@
       <c r="P3" s="8"/>
       <c r="Q3" s="8"/>
       <c r="R3" s="18">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="S3" s="8"/>
       <c r="U3" s="9"/>
@@ -3760,13 +3760,13 @@
         <v>113</v>
       </c>
       <c r="C18" s="15">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="D18" s="15">
         <v>3</v>
       </c>
       <c r="E18" s="15">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="F18" s="15">
         <v>3</v>
@@ -4921,7 +4921,7 @@
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.45" right="0.45" top="0.5" bottom="0.5" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" scale="51" fitToHeight="0" orientation="landscape" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="52" fitToHeight="0" orientation="landscape" r:id="rId1"/>
   <drawing r:id="rId2"/>
   <legacyDrawing r:id="rId3"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -4966,7 +4966,7 @@
       <pane xSplit="8" ySplit="5" topLeftCell="I6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="I1" sqref="I1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
-      <selection pane="bottomRight" activeCell="C12" sqref="C12"/>
+      <selection pane="bottomRight" activeCell="AJ29" sqref="AJ29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.75" defaultRowHeight="17.25" x14ac:dyDescent="0.3"/>
@@ -6007,29 +6007,29 @@
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="47" t="s">
+      <c r="A2" s="46" t="s">
         <v>28</v>
       </c>
       <c r="B2" s="25" t="s">
         <v>39</v>
       </c>
-      <c r="C2" s="50" t="s">
+      <c r="C2" s="49" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="48"/>
+      <c r="A3" s="47"/>
       <c r="B3" s="24" t="s">
         <v>40</v>
       </c>
-      <c r="C3" s="51"/>
+      <c r="C3" s="50"/>
     </row>
     <row r="4" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="49"/>
+      <c r="A4" s="48"/>
       <c r="B4" s="26" t="s">
         <v>41</v>
       </c>
-      <c r="C4" s="52"/>
+      <c r="C4" s="51"/>
     </row>
     <row r="5" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="22" t="s">
@@ -6041,67 +6041,67 @@
       <c r="C5" s="27"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="47" t="s">
+      <c r="A6" s="46" t="s">
         <v>30</v>
       </c>
       <c r="B6" s="25" t="s">
         <v>45</v>
       </c>
-      <c r="C6" s="50" t="s">
+      <c r="C6" s="49" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="48"/>
+      <c r="A7" s="47"/>
       <c r="B7" s="24" t="s">
         <v>46</v>
       </c>
-      <c r="C7" s="51"/>
+      <c r="C7" s="50"/>
     </row>
     <row r="8" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="49"/>
+      <c r="A8" s="48"/>
       <c r="B8" s="26" t="s">
         <v>47</v>
       </c>
-      <c r="C8" s="52"/>
+      <c r="C8" s="51"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="47" t="s">
+      <c r="A9" s="46" t="s">
         <v>31</v>
       </c>
       <c r="B9" s="25" t="s">
         <v>48</v>
       </c>
-      <c r="C9" s="50" t="s">
+      <c r="C9" s="49" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="48"/>
+      <c r="A10" s="47"/>
       <c r="B10" s="24" t="s">
         <v>49</v>
       </c>
-      <c r="C10" s="51"/>
+      <c r="C10" s="50"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" s="48"/>
+      <c r="A11" s="47"/>
       <c r="B11" s="24" t="s">
         <v>50</v>
       </c>
-      <c r="C11" s="51"/>
+      <c r="C11" s="50"/>
       <c r="F11" s="35"/>
       <c r="G11" s="35"/>
-      <c r="H11" s="46" t="s">
+      <c r="H11" s="52" t="s">
         <v>105</v>
       </c>
-      <c r="I11" s="46"/>
+      <c r="I11" s="52"/>
     </row>
     <row r="12" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="49"/>
+      <c r="A12" s="48"/>
       <c r="B12" s="26" t="s">
         <v>51</v>
       </c>
-      <c r="C12" s="52"/>
+      <c r="C12" s="51"/>
       <c r="F12" s="35"/>
       <c r="G12" s="35"/>
       <c r="H12" s="34" t="s">
@@ -6119,7 +6119,7 @@
         <v>74</v>
       </c>
       <c r="C13" s="53"/>
-      <c r="F13" s="46" t="s">
+      <c r="F13" s="52" t="s">
         <v>104</v>
       </c>
       <c r="G13" s="34" t="s">
@@ -6136,7 +6136,7 @@
         <v>75</v>
       </c>
       <c r="C14" s="54"/>
-      <c r="F14" s="46"/>
+      <c r="F14" s="52"/>
       <c r="G14" s="34" t="s">
         <v>101</v>
       </c>
@@ -6176,43 +6176,43 @@
       <c r="C18" s="55"/>
     </row>
     <row r="19" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="47" t="s">
+      <c r="A19" s="46" t="s">
         <v>33</v>
       </c>
       <c r="B19" s="25" t="s">
         <v>80</v>
       </c>
-      <c r="C19" s="50"/>
+      <c r="C19" s="49"/>
     </row>
     <row r="20" spans="1:3" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="49"/>
+      <c r="A20" s="48"/>
       <c r="B20" s="26" t="s">
         <v>81</v>
       </c>
-      <c r="C20" s="52"/>
+      <c r="C20" s="51"/>
     </row>
     <row r="21" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="47" t="s">
+      <c r="A21" s="46" t="s">
         <v>34</v>
       </c>
       <c r="B21" s="25" t="s">
         <v>82</v>
       </c>
-      <c r="C21" s="50"/>
+      <c r="C21" s="49"/>
     </row>
     <row r="22" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="48"/>
+      <c r="A22" s="47"/>
       <c r="B22" s="24" t="s">
         <v>83</v>
       </c>
-      <c r="C22" s="51"/>
+      <c r="C22" s="50"/>
     </row>
     <row r="23" spans="1:3" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="49"/>
+      <c r="A23" s="48"/>
       <c r="B23" s="26" t="s">
         <v>84</v>
       </c>
-      <c r="C23" s="52"/>
+      <c r="C23" s="51"/>
     </row>
     <row r="24" spans="1:3" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="22" t="s">
@@ -6232,59 +6232,53 @@
     <row r="29" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="36" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A37" s="47" t="s">
+      <c r="A37" s="46" t="s">
         <v>53</v>
       </c>
       <c r="B37" s="25" t="s">
         <v>68</v>
       </c>
-      <c r="C37" s="50" t="s">
+      <c r="C37" s="49" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A38" s="48"/>
+      <c r="A38" s="47"/>
       <c r="B38" s="24" t="s">
         <v>69</v>
       </c>
-      <c r="C38" s="51"/>
+      <c r="C38" s="50"/>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A39" s="48"/>
+      <c r="A39" s="47"/>
       <c r="B39" s="24" t="s">
         <v>70</v>
       </c>
-      <c r="C39" s="51"/>
+      <c r="C39" s="50"/>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A40" s="48"/>
+      <c r="A40" s="47"/>
       <c r="B40" s="24" t="s">
         <v>71</v>
       </c>
-      <c r="C40" s="51"/>
+      <c r="C40" s="50"/>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A41" s="48"/>
+      <c r="A41" s="47"/>
       <c r="B41" s="24" t="s">
         <v>72</v>
       </c>
-      <c r="C41" s="51"/>
+      <c r="C41" s="50"/>
     </row>
     <row r="42" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="49"/>
+      <c r="A42" s="48"/>
       <c r="B42" s="26" t="s">
         <v>73</v>
       </c>
-      <c r="C42" s="52"/>
+      <c r="C42" s="51"/>
     </row>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="A2:A4"/>
-    <mergeCell ref="A9:A12"/>
-    <mergeCell ref="A6:A8"/>
-    <mergeCell ref="C9:C12"/>
-    <mergeCell ref="C6:C8"/>
-    <mergeCell ref="C2:C4"/>
     <mergeCell ref="H11:I11"/>
     <mergeCell ref="F13:F14"/>
     <mergeCell ref="A37:A42"/>
@@ -6295,6 +6289,12 @@
     <mergeCell ref="C21:C23"/>
     <mergeCell ref="C13:C18"/>
     <mergeCell ref="A13:A18"/>
+    <mergeCell ref="A2:A4"/>
+    <mergeCell ref="A9:A12"/>
+    <mergeCell ref="A6:A8"/>
+    <mergeCell ref="C9:C12"/>
+    <mergeCell ref="C6:C8"/>
+    <mergeCell ref="C2:C4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="landscape" r:id="rId1"/>

</xml_diff>